<commit_message>
feat: adiciona planilha de dados
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Dados" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Ano</t>
   </si>
@@ -266,16 +267,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="false"/>
-        <i val="false"/>
-        <sz val="10"/>
-        <color rgb="FF0000EE"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>https://www.researchgate.net/publication/389080825_Using_human_mobility_data_to_quantify_experienced_urban_inequalities</t>
-    </r>
+    <t>https://www.researchgate.net/publication/389080825_Using_human_mobility_data_to_quantify_experienced_urban_inequalities</t>
   </si>
   <si>
     <r>
@@ -606,24 +598,8 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="false"/>
-        <i val="false"/>
-        <sz val="10"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>Espaço</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="false"/>
-        <i val="false"/>
-        <sz val="10"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>Tempo</t>
-    </r>
+    <t xml:space="preserve">Espaço
+Tempo</t>
   </si>
   <si>
     <r>
@@ -669,13 +645,55 @@
       </rPr>
       <t>https://journals.sagepub.com/doi/abs/10.1177/0042098020916416</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Análise de deslocamentos dos moradores de assentamentos precários a partir de dados da telefonia móvel em São Paulo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uso de CDR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">São Paulo</t>
+  </si>
+  <si>
+    <t>https://www.teses.usp.br/teses/disponiveis/3/3138/tde-27022018-072715/publico/AndreLeiteRodriguesCorr18.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WorldMove, a global open data for human mobility</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2504.10506</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storm Events Database</t>
+  </si>
+  <si>
+    <t>https://www.ncei.noaa.gov/stormevents/</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The International Disaster Database</t>
+  </si>
+  <si>
+    <t>https://www.emdat.be/</t>
+  </si>
+  <si>
+    <t>Mundial</t>
+  </si>
+  <si>
+    <t>WorldMove</t>
+  </si>
+  <si>
+    <t>https://fi.ee.tsinghua.edu.cn/worldmove/description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -695,6 +713,12 @@
       <u/>
       <sz val="10.000000"/>
       <color rgb="FF0000EE"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10.000000"/>
+      <color theme="10"/>
       <name val="Liberation Sans"/>
     </font>
   </fonts>
@@ -718,8 +742,11 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -762,6 +789,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Default" xfId="0" builtinId="0"/>
@@ -1237,13 +1265,13 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="1" topLeftCell="E1" zoomScale="100" workbookViewId="0">
       <selection activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" width="7.140625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="7.140625"/>
     <col bestFit="1" customWidth="1" min="2" max="2" width="102.140625"/>
     <col bestFit="1" customWidth="1" min="3" max="3" width="25.00390625"/>
     <col bestFit="1" customWidth="1" min="4" max="4" width="20.421875"/>
@@ -1255,274 +1283,301 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" ht="25.5">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>2023</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" ht="38.25">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>2019</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" ht="63.75">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>2025</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" ht="12.75">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="H5" s="11" t="s">
+      <c r="E5" s="11"/>
+      <c r="H5" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" ht="12.75">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="H6" s="11" t="s">
+      <c r="E6" s="11"/>
+      <c r="H6" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" ht="38.25">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>2023</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="12" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" ht="12.75">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>2021</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" ht="12.75">
-      <c r="A9" s="2">
+      <c r="A9" s="3">
         <v>2017</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="11" t="s">
+      <c r="G9" s="13"/>
+      <c r="H9" s="12" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" ht="38.25">
-      <c r="A10" s="2">
+      <c r="A10" s="3">
         <v>2018</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="12" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" ht="12.75">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>2022</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="14" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" ht="12.75">
-      <c r="A12" s="2">
+    <row r="12" ht="25.5">
+      <c r="A12" s="3">
         <v>2020</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" ht="12.75"/>
+    <row r="13" ht="12.75">
+      <c r="A13" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" ht="12.75">
+      <c r="A14" s="1">
+        <v>2025</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="H2"/>
@@ -1536,6 +1591,8 @@
     <hyperlink r:id="rId9" ref="H10"/>
     <hyperlink r:id="rId10" ref="H11"/>
     <hyperlink r:id="rId11" ref="H12"/>
+    <hyperlink r:id="rId12" ref="H13"/>
+    <hyperlink r:id="rId13" ref="H14"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70074299999999978" right="0.70074299999999978" top="1.0518999999999998" bottom="218.411" header="0.78750000000000009" footer="134.99100000000001"/>
@@ -1544,4 +1601,63 @@
     <oddFooter>Página 1</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="30.7109375"/>
+    <col bestFit="1" min="2" max="2" width="43.00390625"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" ht="12.75">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B1"/>
+    <hyperlink r:id="rId2" ref="B2"/>
+    <hyperlink r:id="rId3" ref="B3"/>
+  </hyperlinks>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
docs: inclui novas ideias de titulo e complementa a lista de referências
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Ano</t>
   </si>
@@ -277,43 +277,25 @@
         <sz val="10"/>
         <rFont val="Liberation Sans"/>
       </rPr>
-      <t xml:space="preserve">How do changes in the daily food and transportation environments affect grocery store accessibility?</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="false"/>
-        <i val="false"/>
-        <sz val="10"/>
-        <color rgb="FF0000EE"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>https://www.sciencedirect.com/science/article/pii/S0143622816303721?via%3Dihub</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="false"/>
-        <i val="false"/>
-        <sz val="10"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
       <t xml:space="preserve">Temporal variability in transit-based accessibility to supermarkets</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="false"/>
-        <i val="false"/>
-        <sz val="10"/>
-        <color rgb="FF0000EE"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t>https://www.sciencedirect.com/science/article/pii/S0143622814001283?via%3Dihub</t>
-    </r>
+    <t xml:space="preserve">Dinâmica temporal
+Características sóciodemográficas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matrizes de tempo de viagem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identificação de "food deserts" que mudam de forma dependendo do horário do dia
+Descoberta de disparidades nos níveis médios de acessibilidade com base em raça, renda e idade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cincinnati, Ohio, EUA</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0143622814001283?via%3Dihub</t>
   </si>
   <si>
     <r>
@@ -399,24 +381,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="false"/>
-        <i val="false"/>
-        <sz val="10"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="false"/>
-        <i val="false"/>
-        <sz val="10"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t xml:space="preserve">zonas de baixa renda apresentam índices de caminhabilidade mais alta, mas apresentam menor potencial de acessibilidade para pedestres</t>
-    </r>
+    <t xml:space="preserve">Zonas de baixa renda apresentam índices de caminhabilidade mais alta, mas apresentam menor potencial de acessibilidade para pedestres</t>
   </si>
   <si>
     <r>
@@ -693,7 +658,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -713,6 +678,11 @@
       <u/>
       <sz val="10.000000"/>
       <color rgb="FF0000EE"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
+      <color indexed="64"/>
       <name val="Liberation Sans"/>
     </font>
     <font>
@@ -742,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left"/>
@@ -775,21 +745,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyProtection="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Default" xfId="0" builtinId="0"/>
@@ -1265,7 +1229,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" topLeftCell="E1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="1" topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1386,196 +1350,210 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" ht="12.75">
-      <c r="A5" s="3"/>
+    <row r="5" ht="38.25">
+      <c r="A5" s="3">
+        <v>2014</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="H5" s="12" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="9" t="s">
         <v>29</v>
       </c>
+      <c r="E5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="6" ht="12.75">
-      <c r="A6" s="3"/>
+    <row r="6" ht="38.25">
+      <c r="A6" s="3">
+        <v>2023</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="H6" s="12" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="7" ht="38.25">
+    <row r="7" ht="12.75">
       <c r="A7" s="3">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>36</v>
+      <c r="E7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" ht="12.75">
       <c r="A8" s="3">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>42</v>
+      <c r="E8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="9" ht="12.75">
+    <row r="9" ht="38.25">
       <c r="A9" s="3">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="12" t="s">
-        <v>46</v>
+      <c r="E9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="10" ht="38.25">
+    <row r="10" ht="12.75">
       <c r="A10" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" ht="25.5">
+      <c r="A11" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" ht="12.75">
+      <c r="A12" s="3">
         <v>2018</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" ht="12.75">
-      <c r="A11" s="3">
-        <v>2022</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" ht="25.5">
-      <c r="A12" s="3">
-        <v>2020</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>62</v>
+      <c r="B12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13" ht="12.75">
-      <c r="A13" s="1">
-        <v>2018</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" ht="12.75">
-      <c r="A14" s="1">
+      <c r="A13" s="3">
         <v>2025</v>
       </c>
-      <c r="B14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>68</v>
+      <c r="B13" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="13" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1592,7 +1570,6 @@
     <hyperlink r:id="rId10" ref="H11"/>
     <hyperlink r:id="rId11" ref="H12"/>
     <hyperlink r:id="rId12" ref="H13"/>
-    <hyperlink r:id="rId13" ref="H14"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70074299999999978" right="0.70074299999999978" top="1.0518999999999998" bottom="218.411" header="0.78750000000000009" footer="134.99100000000001"/>
@@ -1618,35 +1595,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" ht="12.75">
       <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
         <v>76</v>
-      </c>
-      <c r="C3" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: adiciona mais referencias e fontes de dados
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0" showHorizontalScroll="1" showVerticalScroll="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1" showHorizontalScroll="1" showVerticalScroll="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Ano</t>
   </si>
@@ -630,6 +630,21 @@
     <t>https://arxiv.org/abs/2504.10506</t>
   </si>
   <si>
+    <t xml:space="preserve">The 15-Minute City Quantified Using Mobility Data</t>
+  </si>
+  <si>
+    <t>https://www.nber.org/system/files/working_papers/w30752/w30752.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pySpainMobility: a Python Package to Access and Manage Spanish Open Mobility Data</t>
+  </si>
+  <si>
+    <t>Espanha</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2506.13385</t>
+  </si>
+  <si>
     <t xml:space="preserve">Storm Events Database</t>
   </si>
   <si>
@@ -652,6 +667,45 @@
   </si>
   <si>
     <t>https://fi.ee.tsinghua.edu.cn/worldmove/description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1746 - Rio</t>
+  </si>
+  <si>
+    <t>https://datariov2-pcrj.hub.arcgis.com/documents/PCRJ::administra%C3%A7%C3%A3o-de-servi%C3%A7os-p%C3%BAblicos-chamados-feitos-ao-1746/about?path=</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUACI - Buenos Aires ("156")</t>
+  </si>
+  <si>
+    <t>https://data.buenosaires.gob.ar/dataset/sistema-unico-atencion-ciudadana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buenos Aires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">156 - São Paulo</t>
+  </si>
+  <si>
+    <t>https://dados.prefeitura.sp.gov.br/dataset/servicos-prestados-pela-pgm-sp156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NetMob (Mobile Phone Data)</t>
+  </si>
+  <si>
+    <t>https://netmob.org/www25/</t>
+  </si>
+  <si>
+    <t>pySpainMobility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SafeGraph / Dewey</t>
+  </si>
+  <si>
+    <t>https://www.deweydata.io/data-partners/safegraph</t>
   </si>
 </sst>
 </file>
@@ -682,7 +736,6 @@
     </font>
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Liberation Sans"/>
     </font>
     <font>
@@ -712,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left"/>
@@ -743,9 +796,6 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
@@ -1229,7 +1279,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView showGridLines="1" topLeftCell="D1" zoomScale="100" workbookViewId="0">
       <selection activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1361,13 +1411,13 @@
       <c r="D5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -1536,7 +1586,7 @@
       <c r="G12" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1552,8 +1602,33 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="12" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="14" ht="12.75">
+      <c r="A14" s="1">
+        <v>2022</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" ht="12.75">
+      <c r="A15" s="1">
+        <v>2025</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1570,6 +1645,8 @@
     <hyperlink r:id="rId10" ref="H11"/>
     <hyperlink r:id="rId11" ref="H12"/>
     <hyperlink r:id="rId12" ref="H13"/>
+    <hyperlink r:id="rId13" ref="H14"/>
+    <hyperlink r:id="rId14" ref="H15"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70074299999999978" right="0.70074299999999978" top="1.0518999999999998" bottom="218.411" header="0.78750000000000009" footer="134.99100000000001"/>
@@ -1590,47 +1667,112 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col bestFit="1" min="1" max="1" width="30.7109375"/>
-    <col bestFit="1" min="2" max="2" width="43.00390625"/>
+    <col bestFit="1" min="2" max="2" width="137.8515625"/>
+    <col bestFit="1" min="3" max="3" width="11.8515625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>72</v>
+        <v>76</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>75</v>
+        <v>79</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" ht="12.75">
       <c r="A3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>78</v>
+        <v>82</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
-      </c>
-    </row>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" ht="12.75">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" ht="12.75">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" ht="12.75">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" ht="12.75">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" ht="12.75"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B1"/>
     <hyperlink r:id="rId2" ref="B2"/>
     <hyperlink r:id="rId3" ref="B3"/>
+    <hyperlink r:id="rId4" ref="B4"/>
+    <hyperlink r:id="rId5" ref="B5"/>
+    <hyperlink r:id="rId6" ref="B6"/>
+    <hyperlink r:id="rId7" ref="B7"/>
+    <hyperlink r:id="rId8" ref="B8"/>
+    <hyperlink r:id="rId9" ref="B9"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
feat: adiciona diagrama draw.io
</commit_message>
<xml_diff>
--- a/references.xlsx
+++ b/references.xlsx
@@ -3,16 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1" showHorizontalScroll="1" showVerticalScroll="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0" showHorizontalScroll="1" showVerticalScroll="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Dados" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
-  </extLst>
 </workbook>
 </file>
 
@@ -136,15 +133,11 @@
 GINI</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b val="false"/>
-        <i val="false"/>
-        <sz val="10"/>
-        <rFont val="Liberation Sans"/>
-      </rPr>
-      <t xml:space="preserve">Cálculo espacial de acessibilidade- Indicador Proximity Time- Indicador F15- Indicador de desigualdade de acessibilidade- Algoritmo de realocação de POIs</t>
-    </r>
+    <t xml:space="preserve">Cálculo espacial de acessibilidade
+Indicador Proximity Time
+Indicador F15
+Indicador de desigualdade de acessibilidade
+Algoritmo de realocação de POIs</t>
   </si>
   <si>
     <r>
@@ -779,14 +772,11 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -799,6 +789,9 @@
     </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
@@ -1355,16 +1348,16 @@
       <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -1381,19 +1374,19 @@
       <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -1407,17 +1400,17 @@
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -1437,10 +1430,10 @@
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="3" t="s">
         <v>37</v>
       </c>
@@ -1461,7 +1454,7 @@
       <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="11" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1487,7 +1480,7 @@
       <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="11" t="s">
         <v>46</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -1505,13 +1498,13 @@
       <c r="B9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>51</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1535,10 +1528,10 @@
         <v>9</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="10"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="3" t="s">
         <v>57</v>
       </c>
@@ -1554,10 +1547,10 @@
         <v>59</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="11" t="s">
         <v>61</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -1574,16 +1567,16 @@
       <c r="A12" s="3">
         <v>2018</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10" t="s">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9" t="s">
         <v>67</v>
       </c>
       <c r="H12" s="12" t="s">
@@ -1594,14 +1587,14 @@
       <c r="A13" s="3">
         <v>2025</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="12" t="s">
         <v>70</v>
       </c>

</xml_diff>